<commit_message>
Re-do TODE grade norms with week coding for grade
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed-grade.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed-grade.xlsx
@@ -379,7 +379,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
@@ -387,7 +387,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4">
@@ -395,7 +395,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
@@ -403,7 +403,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6">
@@ -411,7 +411,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7">
@@ -419,7 +419,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8">
@@ -427,7 +427,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9">
@@ -435,7 +435,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10">
@@ -443,7 +443,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
@@ -451,7 +451,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12">
@@ -459,7 +459,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13">
@@ -467,7 +467,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14">
@@ -475,7 +475,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15">
@@ -483,7 +483,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16">
@@ -491,7 +491,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17">
@@ -499,7 +499,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18">
@@ -507,7 +507,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19">
@@ -515,7 +515,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20">
@@ -523,7 +523,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21">
@@ -531,7 +531,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22">
@@ -539,7 +539,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23">
@@ -547,7 +547,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24">
@@ -555,7 +555,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25">
@@ -563,7 +563,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26">
@@ -571,7 +571,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27">
@@ -579,7 +579,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28">
@@ -587,7 +587,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29">
@@ -595,7 +595,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30">
@@ -668,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
@@ -676,7 +676,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
@@ -684,7 +684,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
@@ -692,7 +692,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
@@ -700,7 +700,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -708,7 +708,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
@@ -716,7 +716,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9">
@@ -724,7 +724,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10">
@@ -732,7 +732,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11">
@@ -740,7 +740,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12">
@@ -748,7 +748,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13">
@@ -756,7 +756,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14">
@@ -764,7 +764,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15">
@@ -772,7 +772,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16">
@@ -780,7 +780,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17">
@@ -788,7 +788,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18">
@@ -796,7 +796,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19">
@@ -820,7 +820,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22">
@@ -828,7 +828,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23">
@@ -836,7 +836,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24">
@@ -844,7 +844,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25">
@@ -852,7 +852,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26">
@@ -860,7 +860,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27">
@@ -868,7 +868,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28">
@@ -876,7 +876,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29">
@@ -884,7 +884,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30">
@@ -892,7 +892,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31">
@@ -900,7 +900,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32">
@@ -908,7 +908,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33">
@@ -916,7 +916,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34">
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -965,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
@@ -973,7 +973,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
@@ -981,7 +981,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
@@ -989,7 +989,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7">
@@ -997,7 +997,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8">
@@ -1005,7 +1005,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
@@ -1013,7 +1013,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10">
@@ -1021,7 +1021,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
@@ -1029,7 +1029,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
@@ -1037,7 +1037,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13">
@@ -1045,7 +1045,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
@@ -1053,7 +1053,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
@@ -1061,7 +1061,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
@@ -1069,7 +1069,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17">
@@ -1077,7 +1077,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
@@ -1085,7 +1085,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
@@ -1101,7 +1101,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21">
@@ -1109,7 +1109,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22">
@@ -1117,7 +1117,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23">
@@ -1125,7 +1125,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24">
@@ -1133,7 +1133,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25">
@@ -1141,7 +1141,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26">
@@ -1149,7 +1149,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27">
@@ -1157,7 +1157,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28">
@@ -1165,7 +1165,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29">
@@ -1173,7 +1173,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30">
@@ -1181,7 +1181,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31">
@@ -1189,7 +1189,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32">
@@ -1197,7 +1197,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33">
@@ -1205,7 +1205,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34">
@@ -1213,7 +1213,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
@@ -1254,7 +1254,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4">
@@ -1262,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
@@ -1270,7 +1270,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>45</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6">
@@ -1278,7 +1278,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7">
@@ -1286,7 +1286,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8">
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>54</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9">
@@ -1302,7 +1302,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10">
@@ -1310,7 +1310,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
@@ -1318,7 +1318,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>62</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12">
@@ -1326,7 +1326,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13">
@@ -1334,7 +1334,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14">
@@ -1342,7 +1342,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15">
@@ -1350,7 +1350,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16">
@@ -1358,7 +1358,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>72</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17">
@@ -1366,7 +1366,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>74</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18">
@@ -1374,7 +1374,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>76</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19">
@@ -1382,7 +1382,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>78</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20">
@@ -1390,7 +1390,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21">
@@ -1398,7 +1398,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>82</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22">
@@ -1406,7 +1406,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>84</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23">
@@ -1414,7 +1414,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>86</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24">
@@ -1422,7 +1422,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>88</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25">
@@ -1430,7 +1430,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>90</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26">
@@ -1438,7 +1438,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27">
@@ -1446,7 +1446,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>94</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28">
@@ -1454,7 +1454,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>97</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29">
@@ -1462,7 +1462,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>99</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30">
@@ -1470,7 +1470,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>102</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31">
@@ -1478,7 +1478,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>104</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32">
@@ -1486,7 +1486,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33">
@@ -1494,7 +1494,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>111</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34">
@@ -1502,7 +1502,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>117</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1575,7 +1575,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8">
@@ -1583,7 +1583,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9">
@@ -1591,7 +1591,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10">
@@ -1599,7 +1599,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11">
@@ -1607,7 +1607,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12">
@@ -1615,7 +1615,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13">
@@ -1623,7 +1623,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -1631,7 +1631,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
@@ -1639,7 +1639,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16">
@@ -1647,7 +1647,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17">
@@ -1655,7 +1655,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
@@ -1663,7 +1663,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
@@ -1671,7 +1671,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20">
@@ -1679,7 +1679,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21">
@@ -1687,7 +1687,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22">
@@ -1695,7 +1695,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23">
@@ -1703,7 +1703,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24">
@@ -1711,7 +1711,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25">
@@ -1719,7 +1719,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26">
@@ -1727,7 +1727,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27">
@@ -1735,7 +1735,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28">
@@ -1743,7 +1743,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29">
@@ -1751,7 +1751,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30">
@@ -1759,7 +1759,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31">
@@ -1767,7 +1767,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32">
@@ -1775,7 +1775,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33">
@@ -1783,7 +1783,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34">
@@ -1791,7 +1791,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1888,7 +1888,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11">
@@ -1896,7 +1896,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
@@ -1904,7 +1904,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
@@ -1912,7 +1912,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14">
@@ -1920,7 +1920,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
@@ -1928,7 +1928,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16">
@@ -1936,7 +1936,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17">
@@ -1944,7 +1944,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18">
@@ -1952,7 +1952,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19">
@@ -1960,7 +1960,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20">
@@ -1968,7 +1968,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21">
@@ -1976,7 +1976,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22">
@@ -1984,7 +1984,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23">
@@ -1992,7 +1992,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24">
@@ -2000,7 +2000,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25">
@@ -2008,7 +2008,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26">
@@ -2016,7 +2016,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27">
@@ -2024,7 +2024,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28">
@@ -2032,7 +2032,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29">
@@ -2040,7 +2040,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30">
@@ -2048,7 +2048,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31">
@@ -2056,7 +2056,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32">
@@ -2064,7 +2064,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33">
@@ -2072,7 +2072,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34">

</xml_diff>

<commit_message>
Finish re run of TODE grade norms
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed-grade.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed-grade.xlsx
@@ -356,7 +356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -376,265 +376,433 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>-20</v>
       </c>
       <c r="B2">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>-19</v>
       </c>
       <c r="B3">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>-18</v>
       </c>
       <c r="B4">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>-17</v>
       </c>
       <c r="B5">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>-16</v>
       </c>
       <c r="B6">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>-15</v>
       </c>
       <c r="B7">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>-14</v>
       </c>
       <c r="B8">
-        <v>74</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>-13</v>
       </c>
       <c r="B9">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>-12</v>
       </c>
       <c r="B10">
-        <v>79</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>-11</v>
       </c>
       <c r="B11">
-        <v>81</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>-10</v>
       </c>
       <c r="B12">
-        <v>84</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>-9</v>
       </c>
       <c r="B13">
-        <v>86</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>-8</v>
       </c>
       <c r="B14">
-        <v>89</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>-7</v>
       </c>
       <c r="B15">
-        <v>91</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>-6</v>
       </c>
       <c r="B16">
-        <v>94</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>-5</v>
       </c>
       <c r="B17">
-        <v>96</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>-4</v>
       </c>
       <c r="B18">
-        <v>99</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>-3</v>
       </c>
       <c r="B19">
-        <v>101</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>-2</v>
       </c>
       <c r="B20">
-        <v>104</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>-1</v>
       </c>
       <c r="B21">
-        <v>106</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>109</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>111</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>114</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>116</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>119</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>121</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B28">
-        <v>124</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B29">
-        <v>126</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B30">
-        <v>129</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B31">
-        <v>130</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B32">
-        <v>130</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B33">
-        <v>130</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>16</v>
+      </c>
+      <c r="B38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>18</v>
+      </c>
+      <c r="B40">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>21</v>
+      </c>
+      <c r="B43">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>22</v>
+      </c>
+      <c r="B44">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>26</v>
+      </c>
+      <c r="B48">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>27</v>
+      </c>
+      <c r="B49">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>28</v>
+      </c>
+      <c r="B50">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>29</v>
+      </c>
+      <c r="B51">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>30</v>
+      </c>
+      <c r="B52">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>31</v>
+      </c>
+      <c r="B53">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>32</v>
+      </c>
+      <c r="B54">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B55">
         <v>130</v>
       </c>
     </row>
@@ -645,7 +813,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -665,266 +833,434 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>-20</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>-19</v>
       </c>
       <c r="B3">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>-18</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>-17</v>
       </c>
       <c r="B5">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>-16</v>
       </c>
       <c r="B6">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>-15</v>
       </c>
       <c r="B7">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>-14</v>
       </c>
       <c r="B8">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>-13</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>-12</v>
       </c>
       <c r="B10">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>-11</v>
       </c>
       <c r="B11">
-        <v>74</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>-10</v>
       </c>
       <c r="B12">
-        <v>76</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>-9</v>
       </c>
       <c r="B13">
-        <v>79</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>-8</v>
       </c>
       <c r="B14">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>-7</v>
       </c>
       <c r="B15">
-        <v>84</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>-6</v>
       </c>
       <c r="B16">
-        <v>86</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>-5</v>
       </c>
       <c r="B17">
-        <v>89</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>-4</v>
       </c>
       <c r="B18">
-        <v>91</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>-3</v>
       </c>
       <c r="B19">
-        <v>94</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>-2</v>
       </c>
       <c r="B20">
-        <v>96</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>-1</v>
       </c>
       <c r="B21">
-        <v>99</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>101</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>104</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>106</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>109</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>111</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>114</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B28">
-        <v>116</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B29">
-        <v>119</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B30">
-        <v>121</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B31">
-        <v>124</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B32">
-        <v>126</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B33">
-        <v>129</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>16</v>
+      </c>
+      <c r="B38">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>18</v>
+      </c>
+      <c r="B40">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>21</v>
+      </c>
+      <c r="B43">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>22</v>
+      </c>
+      <c r="B44">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>26</v>
+      </c>
+      <c r="B48">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>27</v>
+      </c>
+      <c r="B49">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>28</v>
+      </c>
+      <c r="B50">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>29</v>
+      </c>
+      <c r="B51">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>30</v>
+      </c>
+      <c r="B52">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>31</v>
+      </c>
+      <c r="B53">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>32</v>
+      </c>
+      <c r="B54">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>130</v>
+      <c r="B55">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -934,7 +1270,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -954,266 +1290,434 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>-20</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>-19</v>
       </c>
       <c r="B3">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>-18</v>
       </c>
       <c r="B4">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>-17</v>
       </c>
       <c r="B5">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>-16</v>
       </c>
       <c r="B6">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>-15</v>
       </c>
       <c r="B7">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>-14</v>
       </c>
       <c r="B8">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>-13</v>
       </c>
       <c r="B9">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>-12</v>
       </c>
       <c r="B10">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>-11</v>
       </c>
       <c r="B11">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>-10</v>
       </c>
       <c r="B12">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>-9</v>
       </c>
       <c r="B13">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>-8</v>
       </c>
       <c r="B14">
-        <v>74</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>-7</v>
       </c>
       <c r="B15">
-        <v>76</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>-6</v>
       </c>
       <c r="B16">
-        <v>79</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>-5</v>
       </c>
       <c r="B17">
-        <v>81</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>-4</v>
       </c>
       <c r="B18">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>-3</v>
       </c>
       <c r="B19">
-        <v>86</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>-2</v>
       </c>
       <c r="B20">
-        <v>89</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>-1</v>
       </c>
       <c r="B21">
-        <v>91</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>94</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>96</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>99</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>101</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>104</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>106</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B28">
-        <v>109</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B29">
-        <v>111</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B30">
-        <v>114</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B31">
-        <v>116</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B32">
-        <v>119</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B33">
-        <v>121</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>16</v>
+      </c>
+      <c r="B38">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>18</v>
+      </c>
+      <c r="B40">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>21</v>
+      </c>
+      <c r="B43">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>22</v>
+      </c>
+      <c r="B44">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>26</v>
+      </c>
+      <c r="B48">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>27</v>
+      </c>
+      <c r="B49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>28</v>
+      </c>
+      <c r="B50">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>29</v>
+      </c>
+      <c r="B51">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>30</v>
+      </c>
+      <c r="B52">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>31</v>
+      </c>
+      <c r="B53">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>32</v>
+      </c>
+      <c r="B54">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>124</v>
+      <c r="B55">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1727,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1243,265 +1747,433 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>-20</v>
       </c>
       <c r="B2">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>-19</v>
       </c>
       <c r="B3">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>-18</v>
       </c>
       <c r="B4">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>-17</v>
       </c>
       <c r="B5">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>-16</v>
       </c>
       <c r="B6">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>-15</v>
       </c>
       <c r="B7">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>-14</v>
       </c>
       <c r="B8">
-        <v>74</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>-13</v>
       </c>
       <c r="B9">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>-12</v>
       </c>
       <c r="B10">
-        <v>79</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>-11</v>
       </c>
       <c r="B11">
-        <v>81</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>-10</v>
       </c>
       <c r="B12">
-        <v>84</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>-9</v>
       </c>
       <c r="B13">
-        <v>86</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>-8</v>
       </c>
       <c r="B14">
-        <v>89</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>-7</v>
       </c>
       <c r="B15">
-        <v>91</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>-6</v>
       </c>
       <c r="B16">
-        <v>94</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>-5</v>
       </c>
       <c r="B17">
-        <v>96</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>-4</v>
       </c>
       <c r="B18">
-        <v>99</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>-3</v>
       </c>
       <c r="B19">
-        <v>101</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>-2</v>
       </c>
       <c r="B20">
-        <v>104</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>-1</v>
       </c>
       <c r="B21">
-        <v>106</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>109</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>111</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>114</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>116</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>119</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>121</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B28">
-        <v>124</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B29">
-        <v>126</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B30">
-        <v>129</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B31">
-        <v>130</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B32">
-        <v>130</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B33">
-        <v>130</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>16</v>
+      </c>
+      <c r="B38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>18</v>
+      </c>
+      <c r="B40">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>21</v>
+      </c>
+      <c r="B43">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>22</v>
+      </c>
+      <c r="B44">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>26</v>
+      </c>
+      <c r="B48">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>27</v>
+      </c>
+      <c r="B49">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>28</v>
+      </c>
+      <c r="B50">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>29</v>
+      </c>
+      <c r="B51">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>30</v>
+      </c>
+      <c r="B52">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>31</v>
+      </c>
+      <c r="B53">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>32</v>
+      </c>
+      <c r="B54">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B55">
         <v>130</v>
       </c>
     </row>
@@ -1512,7 +2184,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1532,7 +2204,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>-20</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -1540,7 +2212,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>-19</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -1548,7 +2220,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>-18</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -1556,7 +2228,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>-17</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -1564,7 +2236,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>-16</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -1572,226 +2244,394 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>-15</v>
       </c>
       <c r="B7">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>-14</v>
       </c>
       <c r="B8">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>-13</v>
       </c>
       <c r="B9">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>-12</v>
       </c>
       <c r="B10">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>-11</v>
       </c>
       <c r="B11">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>-10</v>
       </c>
       <c r="B12">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>-9</v>
       </c>
       <c r="B13">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>-8</v>
       </c>
       <c r="B14">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>-7</v>
       </c>
       <c r="B15">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>-6</v>
       </c>
       <c r="B16">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>-5</v>
       </c>
       <c r="B17">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>-4</v>
       </c>
       <c r="B18">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>-3</v>
       </c>
       <c r="B19">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>-2</v>
       </c>
       <c r="B20">
-        <v>74</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>-1</v>
       </c>
       <c r="B21">
-        <v>76</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>79</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>81</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>86</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>89</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>91</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B28">
-        <v>94</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B29">
-        <v>96</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B30">
-        <v>99</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B31">
-        <v>101</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B32">
-        <v>104</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B33">
-        <v>106</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>16</v>
+      </c>
+      <c r="B38">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>18</v>
+      </c>
+      <c r="B40">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>21</v>
+      </c>
+      <c r="B43">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>22</v>
+      </c>
+      <c r="B44">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>26</v>
+      </c>
+      <c r="B48">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>27</v>
+      </c>
+      <c r="B49">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>28</v>
+      </c>
+      <c r="B50">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>29</v>
+      </c>
+      <c r="B51">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>30</v>
+      </c>
+      <c r="B52">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>31</v>
+      </c>
+      <c r="B53">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>32</v>
+      </c>
+      <c r="B54">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>109</v>
+      <c r="B55">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1801,7 +2641,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1821,7 +2661,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>-20</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -1829,7 +2669,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>-19</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -1837,7 +2677,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>-18</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -1845,7 +2685,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>-17</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -1853,7 +2693,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>-16</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -1861,7 +2701,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>-15</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -1869,7 +2709,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>-14</v>
       </c>
       <c r="B8">
         <v>40</v>
@@ -1877,7 +2717,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>-13</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -1885,202 +2725,370 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>-12</v>
       </c>
       <c r="B10">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>-11</v>
       </c>
       <c r="B11">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>-10</v>
       </c>
       <c r="B12">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>-9</v>
       </c>
       <c r="B13">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>-8</v>
       </c>
       <c r="B14">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>-7</v>
       </c>
       <c r="B15">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>-6</v>
       </c>
       <c r="B16">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>-5</v>
       </c>
       <c r="B17">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>-4</v>
       </c>
       <c r="B18">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>-3</v>
       </c>
       <c r="B19">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>-2</v>
       </c>
       <c r="B20">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>20</v>
+        <v>-1</v>
       </c>
       <c r="B21">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>74</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>76</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>79</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>81</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B28">
-        <v>86</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B29">
-        <v>89</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B30">
-        <v>91</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B31">
-        <v>94</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B32">
-        <v>96</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B33">
-        <v>99</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>16</v>
+      </c>
+      <c r="B38">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>18</v>
+      </c>
+      <c r="B40">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>21</v>
+      </c>
+      <c r="B43">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>22</v>
+      </c>
+      <c r="B44">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>26</v>
+      </c>
+      <c r="B48">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>27</v>
+      </c>
+      <c r="B49">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>28</v>
+      </c>
+      <c r="B50">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>29</v>
+      </c>
+      <c r="B51">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>30</v>
+      </c>
+      <c r="B52">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>31</v>
+      </c>
+      <c r="B53">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>32</v>
+      </c>
+      <c r="B54">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>101</v>
+      <c r="B55">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rerun all TODE norms, found error in grade code that was creating the wierd column
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed-grade.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed-grade.xlsx
@@ -379,7 +379,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
@@ -387,7 +387,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4">
@@ -395,7 +395,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -403,7 +403,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6">
@@ -411,7 +411,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7">
@@ -419,7 +419,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
@@ -427,7 +427,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9">
@@ -435,7 +435,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
@@ -443,7 +443,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11">
@@ -451,7 +451,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12">
@@ -459,7 +459,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13">
@@ -483,7 +483,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16">
@@ -491,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17">
@@ -499,7 +499,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18">
@@ -507,7 +507,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19">
@@ -515,7 +515,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20">
@@ -523,7 +523,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21">
@@ -531,7 +531,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22">
@@ -539,7 +539,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23">
@@ -547,7 +547,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24">
@@ -555,7 +555,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25">
@@ -563,7 +563,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26">
@@ -571,7 +571,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27">
@@ -579,7 +579,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28">
@@ -587,7 +587,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29">
@@ -595,7 +595,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30">
@@ -603,7 +603,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31">
@@ -611,7 +611,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32">
@@ -619,7 +619,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33">
@@ -627,7 +627,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34">
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3">
@@ -684,7 +684,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
@@ -692,7 +692,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
@@ -700,7 +700,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6">
@@ -708,7 +708,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
@@ -716,7 +716,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8">
@@ -724,7 +724,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9">
@@ -732,7 +732,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10">
@@ -740,7 +740,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11">
@@ -748,7 +748,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12">
@@ -756,7 +756,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13">
@@ -764,7 +764,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
@@ -772,7 +772,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15">
@@ -780,7 +780,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
@@ -788,7 +788,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17">
@@ -796,7 +796,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18">
@@ -836,7 +836,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
@@ -844,7 +844,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24">
@@ -852,7 +852,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25">
@@ -860,7 +860,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26">
@@ -868,7 +868,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27">
@@ -876,7 +876,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
@@ -884,7 +884,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29">
@@ -892,7 +892,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30">
@@ -900,7 +900,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31">
@@ -908,7 +908,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32">
@@ -924,7 +924,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34">
@@ -932,7 +932,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35">
@@ -940,7 +940,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -973,7 +973,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
@@ -981,7 +981,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -989,7 +989,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">
@@ -997,7 +997,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
@@ -1005,7 +1005,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7">
@@ -1013,7 +1013,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
@@ -1021,7 +1021,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
@@ -1029,7 +1029,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10">
@@ -1037,7 +1037,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11">
@@ -1045,7 +1045,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12">
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
@@ -1061,7 +1061,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
@@ -1069,7 +1069,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
@@ -1077,7 +1077,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
@@ -1085,7 +1085,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17">
@@ -1093,7 +1093,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
@@ -1101,7 +1101,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19">
@@ -1109,7 +1109,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
@@ -1117,7 +1117,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
@@ -1125,7 +1125,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22">
@@ -1149,7 +1149,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25">
@@ -1157,7 +1157,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26">
@@ -1165,7 +1165,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27">
@@ -1173,7 +1173,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28">
@@ -1181,7 +1181,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29">
@@ -1189,7 +1189,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30">
@@ -1197,7 +1197,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31">
@@ -1205,7 +1205,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32">
@@ -1213,7 +1213,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33">
@@ -1221,7 +1221,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34">
@@ -1237,7 +1237,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1270,7 +1270,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -1278,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -1286,7 +1286,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>73</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -1294,7 +1294,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>75</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6">
@@ -1302,7 +1302,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7">
@@ -1310,7 +1310,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>79</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8">
@@ -1318,7 +1318,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>81</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9">
@@ -1326,7 +1326,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>83</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10">
@@ -1334,7 +1334,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>84</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
@@ -1342,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>86</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12">
@@ -1350,7 +1350,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>88</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13">
@@ -1358,7 +1358,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>90</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
@@ -1366,7 +1366,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>92</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -1374,7 +1374,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>94</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
@@ -1382,7 +1382,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17">
@@ -1390,7 +1390,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>98</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18">
@@ -1398,7 +1398,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19">
@@ -1406,7 +1406,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>102</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20">
@@ -1414,7 +1414,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21">
@@ -1422,7 +1422,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>106</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22">
@@ -1430,7 +1430,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23">
@@ -1438,7 +1438,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24">
@@ -1446,7 +1446,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>112</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25">
@@ -1454,7 +1454,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>114</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26">
@@ -1462,7 +1462,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>116</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27">
@@ -1470,7 +1470,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>118</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28">
@@ -1478,7 +1478,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>120</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29">
@@ -1486,7 +1486,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>122</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30">
@@ -1494,7 +1494,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>124</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31">
@@ -1502,7 +1502,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>126</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32">
@@ -1510,7 +1510,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>128</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33">
@@ -1518,7 +1518,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>129</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34">
@@ -1526,7 +1526,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>130</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35">
@@ -1534,7 +1534,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>130</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1623,7 +1623,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -1631,7 +1631,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -1647,7 +1647,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -1655,7 +1655,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14">
@@ -1663,7 +1663,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15">
@@ -1671,7 +1671,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16">
@@ -1679,7 +1679,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17">
@@ -1687,7 +1687,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18">
@@ -1695,7 +1695,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19">
@@ -1703,7 +1703,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20">
@@ -1711,7 +1711,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21">
@@ -1719,7 +1719,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22">
@@ -1727,7 +1727,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23">
@@ -1735,7 +1735,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24">
@@ -1743,7 +1743,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25">
@@ -1751,7 +1751,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26">
@@ -1759,7 +1759,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27">
@@ -1783,7 +1783,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30">
@@ -1791,7 +1791,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31">
@@ -1799,7 +1799,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32">
@@ -1807,7 +1807,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33">
@@ -1815,7 +1815,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34">
@@ -1823,7 +1823,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35">
@@ -1831,7 +1831,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1968,7 +1968,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16">
@@ -1984,7 +1984,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18">
@@ -1992,7 +1992,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19">
@@ -2000,7 +2000,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20">
@@ -2008,7 +2008,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21">
@@ -2016,7 +2016,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22">
@@ -2024,7 +2024,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23">
@@ -2032,7 +2032,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24">
@@ -2040,7 +2040,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25">
@@ -2048,7 +2048,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26">
@@ -2056,7 +2056,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27">
@@ -2064,7 +2064,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28">
@@ -2072,7 +2072,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29">
@@ -2080,7 +2080,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30">
@@ -2096,7 +2096,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32">
@@ -2104,7 +2104,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33">
@@ -2112,7 +2112,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34">
@@ -2120,7 +2120,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35">
@@ -2128,7 +2128,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>